<commit_message>
fixed spreadsheet for spring 2019
There were two versions of the spring 2019 spreadsheet; neither one was complete.  Now there is one, and it is correct, I think.
</commit_message>
<xml_diff>
--- a/StudentGuideModule1/what_labs_to_include/131 lab list for 2019spring.xlsx
+++ b/StudentGuideModule1/what_labs_to_include/131 lab list for 2019spring.xlsx
@@ -25,7 +25,7 @@
     <author>Matt Trawick</author>
   </authors>
   <commentList>
-    <comment ref="U1" authorId="0" shapeId="0">
+    <comment ref="V1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V11" authorId="0" shapeId="0">
+    <comment ref="W11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W19" authorId="0" shapeId="0">
+    <comment ref="X19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U22" authorId="0" shapeId="0">
+    <comment ref="V22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -126,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V22" authorId="0" shapeId="0">
+    <comment ref="W22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -150,7 +150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X22" authorId="0" shapeId="0">
+    <comment ref="Y22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -180,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="193">
   <si>
     <t>1 Music to Our Ears: Standing Waves in Strings 7</t>
   </si>
@@ -729,15 +729,9 @@
     <t>ipads</t>
   </si>
   <si>
-    <t>Force by Matt</t>
-  </si>
-  <si>
     <t>2018 fall Jerry</t>
   </si>
   <si>
-    <t>2018 fall Patrick</t>
-  </si>
-  <si>
     <t>2018 fall Mariama</t>
   </si>
   <si>
@@ -760,6 +754,15 @@
   </si>
   <si>
     <t>New, by Christine, 2018</t>
+  </si>
+  <si>
+    <t>2019 spr Patrick</t>
+  </si>
+  <si>
+    <t>2019 spr Shaun</t>
+  </si>
+  <si>
+    <t>Force by editor</t>
   </si>
 </sst>
 </file>
@@ -2016,10 +2019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB113"/>
+  <dimension ref="A1:AC113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V54" sqref="V54"/>
+    <sheetView tabSelected="1" topLeftCell="D61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R78" sqref="R78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2033,16 +2036,16 @@
     <col min="11" max="12" width="8.77734375" style="2" customWidth="1"/>
     <col min="13" max="13" width="8.77734375" style="20" customWidth="1"/>
     <col min="14" max="14" width="10.21875" style="36" customWidth="1"/>
-    <col min="15" max="17" width="8.77734375" style="36" customWidth="1"/>
-    <col min="18" max="18" width="8.77734375" style="2" customWidth="1"/>
-    <col min="19" max="19" width="11" style="3" customWidth="1"/>
-    <col min="20" max="20" width="2.44140625" style="3" customWidth="1"/>
-    <col min="21" max="21" width="10.33203125" style="3" customWidth="1"/>
-    <col min="23" max="23" width="9.5546875" customWidth="1"/>
-    <col min="24" max="24" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="8.77734375" style="36" customWidth="1"/>
+    <col min="19" max="19" width="8.77734375" style="2" customWidth="1"/>
+    <col min="20" max="20" width="11" style="3" customWidth="1"/>
+    <col min="21" max="21" width="2.44140625" style="3" customWidth="1"/>
+    <col min="22" max="22" width="10.33203125" style="3" customWidth="1"/>
+    <col min="24" max="24" width="9.5546875" customWidth="1"/>
+    <col min="25" max="25" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>73</v>
       </c>
@@ -2083,34 +2086,37 @@
         <v>179</v>
       </c>
       <c r="N1" s="49" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="O1" s="49" t="s">
+        <v>181</v>
+      </c>
+      <c r="P1" s="49" t="s">
         <v>182</v>
       </c>
-      <c r="P1" s="49" t="s">
-        <v>184</v>
-      </c>
       <c r="Q1" s="49" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="R1" s="49" t="s">
-        <v>181</v>
-      </c>
-      <c r="S1" s="52" t="s">
-        <v>188</v>
-      </c>
-      <c r="T1" s="32"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="32"/>
+        <v>191</v>
+      </c>
+      <c r="S1" s="49" t="s">
+        <v>192</v>
+      </c>
+      <c r="T1" s="52" t="s">
+        <v>186</v>
+      </c>
+      <c r="U1" s="32"/>
+      <c r="V1" s="33"/>
       <c r="W1" s="32"/>
       <c r="X1" s="32"/>
-      <c r="Y1" s="33"/>
+      <c r="Y1" s="32"/>
       <c r="Z1" s="33"/>
       <c r="AA1" s="33"/>
       <c r="AB1" s="33"/>
-    </row>
-    <row r="2" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AC1" s="33"/>
+    </row>
+    <row r="2" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>86</v>
       </c>
@@ -2148,22 +2154,25 @@
       <c r="Q2" s="59">
         <v>1</v>
       </c>
-      <c r="R2" s="55"/>
-      <c r="S2" s="75">
-        <f>SUM(N2:R2)</f>
-        <v>3</v>
-      </c>
-      <c r="T2" s="80"/>
+      <c r="R2" s="59">
+        <v>1</v>
+      </c>
+      <c r="S2" s="55"/>
+      <c r="T2" s="75">
+        <f>SUM(Q2:S2)</f>
+        <v>2</v>
+      </c>
       <c r="U2" s="80"/>
       <c r="V2" s="80"/>
       <c r="W2" s="80"/>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="33"/>
+      <c r="X2" s="80"/>
+      <c r="Y2" s="32"/>
       <c r="Z2" s="33"/>
       <c r="AA2" s="33"/>
       <c r="AB2" s="33"/>
-    </row>
-    <row r="3" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AC2" s="33"/>
+    </row>
+    <row r="3" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="48"/>
       <c r="B3" s="54" t="s">
         <v>88</v>
@@ -2199,22 +2208,25 @@
       <c r="Q3" s="60">
         <v>1</v>
       </c>
-      <c r="R3" s="60"/>
-      <c r="S3" s="76">
-        <f t="shared" ref="S3:S67" si="0">SUM(N3:R3)</f>
-        <v>3</v>
-      </c>
-      <c r="T3" s="80"/>
+      <c r="R3" s="60">
+        <v>1</v>
+      </c>
+      <c r="S3" s="60"/>
+      <c r="T3" s="76">
+        <f t="shared" ref="T3:T66" si="0">SUM(Q3:S3)</f>
+        <v>2</v>
+      </c>
       <c r="U3" s="80"/>
       <c r="V3" s="80"/>
       <c r="W3" s="80"/>
-      <c r="X3" s="32"/>
-      <c r="Y3" s="33"/>
+      <c r="X3" s="80"/>
+      <c r="Y3" s="32"/>
       <c r="Z3" s="33"/>
       <c r="AA3" s="33"/>
       <c r="AB3" s="33"/>
-    </row>
-    <row r="4" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AC3" s="33"/>
+    </row>
+    <row r="4" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>110</v>
       </c>
@@ -2259,21 +2271,22 @@
         <v>1</v>
       </c>
       <c r="R4" s="36"/>
-      <c r="S4" s="77">
-        <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-      <c r="T4" s="5"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="33"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="15"/>
       <c r="Z4" s="33"/>
       <c r="AA4" s="33"/>
       <c r="AB4" s="33"/>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC4" s="33"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
         <v>120</v>
       </c>
@@ -2287,22 +2300,22 @@
       <c r="L5" s="2">
         <v>0.75</v>
       </c>
-      <c r="R5" s="34"/>
-      <c r="S5" s="77">
+      <c r="S5" s="34"/>
+      <c r="T5" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T5" s="5"/>
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
       <c r="W5" s="5"/>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="33"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="15"/>
       <c r="Z5" s="33"/>
       <c r="AA5" s="33"/>
       <c r="AB5" s="33"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC5" s="33"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" s="30"/>
       <c r="B6" s="31" t="s">
         <v>121</v>
@@ -2316,22 +2329,22 @@
         <v>0</v>
       </c>
       <c r="M6" s="36"/>
-      <c r="R6" s="36"/>
-      <c r="S6" s="77">
+      <c r="S6" s="36"/>
+      <c r="T6" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T6" s="5"/>
       <c r="U6" s="5"/>
       <c r="V6" s="5"/>
       <c r="W6" s="5"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="33"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="15"/>
       <c r="Z6" s="33"/>
       <c r="AA6" s="33"/>
       <c r="AB6" s="33"/>
-    </row>
-    <row r="7" spans="1:28" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AC6" s="33"/>
+    </row>
+    <row r="7" spans="1:29" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="23" t="s">
         <v>122</v>
@@ -2355,18 +2368,19 @@
       <c r="O7" s="36"/>
       <c r="P7" s="36"/>
       <c r="Q7" s="36"/>
-      <c r="R7" s="34"/>
-      <c r="S7" s="77">
+      <c r="R7" s="36"/>
+      <c r="S7" s="34"/>
+      <c r="T7" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T7" s="5"/>
       <c r="U7" s="5"/>
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
-      <c r="X7" s="15"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="X7" s="5"/>
+      <c r="Y7" s="15"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B8" s="23" t="s">
         <v>123</v>
       </c>
@@ -2377,22 +2391,22 @@
       <c r="L8" s="2">
         <v>0</v>
       </c>
-      <c r="R8" s="34"/>
-      <c r="S8" s="77">
+      <c r="S8" s="34"/>
+      <c r="T8" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T8" s="5"/>
       <c r="U8" s="5"/>
       <c r="V8" s="5"/>
       <c r="W8" s="5"/>
-      <c r="X8" s="15"/>
-      <c r="Y8" s="33"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="15"/>
       <c r="Z8" s="33"/>
       <c r="AA8" s="33"/>
       <c r="AB8" s="33"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC8" s="33"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B9" s="23" t="s">
         <v>124</v>
       </c>
@@ -2430,22 +2444,25 @@
       <c r="Q9" s="36">
         <v>1</v>
       </c>
-      <c r="R9" s="34"/>
-      <c r="S9" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T9" s="5"/>
+      <c r="R9" s="36">
+        <v>1</v>
+      </c>
+      <c r="S9" s="34"/>
+      <c r="T9" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="U9" s="5"/>
       <c r="V9" s="5"/>
       <c r="W9" s="5"/>
-      <c r="X9" s="15"/>
-      <c r="Y9" s="33"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="15"/>
       <c r="Z9" s="33"/>
       <c r="AA9" s="33"/>
       <c r="AB9" s="33"/>
-    </row>
-    <row r="10" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AC9" s="33"/>
+    </row>
+    <row r="10" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="23" t="s">
         <v>125</v>
       </c>
@@ -2483,22 +2500,25 @@
       <c r="Q10" s="36">
         <v>1</v>
       </c>
-      <c r="R10" s="34"/>
-      <c r="S10" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T10" s="5"/>
+      <c r="R10" s="36">
+        <v>1</v>
+      </c>
+      <c r="S10" s="34"/>
+      <c r="T10" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="U10" s="5"/>
       <c r="V10" s="5"/>
       <c r="W10" s="5"/>
-      <c r="X10" s="15"/>
-      <c r="Y10" s="33"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="15"/>
       <c r="Z10" s="33"/>
       <c r="AA10" s="33"/>
       <c r="AB10" s="33"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC10" s="33"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B11" s="23" t="s">
         <v>126</v>
       </c>
@@ -2533,24 +2553,27 @@
       <c r="Q11" s="36">
         <v>1</v>
       </c>
-      <c r="R11" s="34"/>
-      <c r="S11" s="77">
-        <f t="shared" si="0"/>
-        <v>2.75</v>
-      </c>
-      <c r="T11" s="5"/>
-      <c r="U11" s="42" t="s">
+      <c r="R11" s="36">
+        <v>1</v>
+      </c>
+      <c r="S11" s="34"/>
+      <c r="T11" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U11" s="5"/>
+      <c r="V11" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="V11" s="43"/>
-      <c r="W11" s="5"/>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="33"/>
+      <c r="W11" s="43"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="15"/>
       <c r="Z11" s="33"/>
       <c r="AA11" s="33"/>
       <c r="AB11" s="33"/>
-    </row>
-    <row r="12" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AC11" s="33"/>
+    </row>
+    <row r="12" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="23" t="s">
         <v>127</v>
       </c>
@@ -2563,24 +2586,24 @@
         <v>0</v>
       </c>
       <c r="M12" s="36"/>
-      <c r="R12" s="34"/>
-      <c r="S12" s="77">
+      <c r="S12" s="34"/>
+      <c r="T12" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T12" s="15"/>
-      <c r="U12" s="44">
+      <c r="U12" s="15"/>
+      <c r="V12" s="44">
         <v>1.5</v>
       </c>
-      <c r="V12" s="45"/>
-      <c r="W12" s="5"/>
-      <c r="X12" s="15"/>
-      <c r="Y12" s="33"/>
+      <c r="W12" s="45"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="15"/>
       <c r="Z12" s="33"/>
       <c r="AA12" s="33"/>
       <c r="AB12" s="33"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC12" s="33"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B13" s="23" t="s">
         <v>175</v>
       </c>
@@ -2615,22 +2638,25 @@
       <c r="Q13" s="36">
         <v>1</v>
       </c>
-      <c r="R13" s="34"/>
-      <c r="S13" s="77">
+      <c r="R13" s="36">
+        <v>1</v>
+      </c>
+      <c r="S13" s="34"/>
+      <c r="T13" s="77">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="T13" s="5"/>
-      <c r="U13" s="33"/>
+      <c r="U13" s="5"/>
       <c r="V13" s="33"/>
-      <c r="W13" s="5"/>
-      <c r="X13" s="15"/>
-      <c r="Y13" s="33"/>
+      <c r="W13" s="33"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="15"/>
       <c r="Z13" s="33"/>
       <c r="AA13" s="33"/>
       <c r="AB13" s="33"/>
-    </row>
-    <row r="14" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AC13" s="33"/>
+    </row>
+    <row r="14" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="23" t="s">
         <v>128</v>
       </c>
@@ -2665,23 +2691,26 @@
       <c r="Q14" s="36">
         <v>1</v>
       </c>
-      <c r="R14" s="34"/>
-      <c r="S14" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T14" s="5"/>
-      <c r="U14" s="1" t="s">
+      <c r="R14" s="36">
+        <v>1</v>
+      </c>
+      <c r="S14" s="34"/>
+      <c r="T14" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U14" s="5"/>
+      <c r="V14" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="W14" s="33"/>
-      <c r="X14" s="15"/>
-      <c r="Y14" s="33"/>
+      <c r="X14" s="33"/>
+      <c r="Y14" s="15"/>
       <c r="Z14" s="33"/>
       <c r="AA14" s="33"/>
       <c r="AB14" s="33"/>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC14" s="33"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B15" s="23" t="s">
         <v>174</v>
       </c>
@@ -2697,26 +2726,26 @@
         <v>0</v>
       </c>
       <c r="M15" s="36"/>
-      <c r="R15" s="34"/>
-      <c r="S15" s="77">
+      <c r="S15" s="34"/>
+      <c r="T15" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T15" s="5"/>
-      <c r="U15" s="17" t="s">
+      <c r="U15" s="5"/>
+      <c r="V15" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="V15" s="38"/>
-      <c r="W15" s="16">
+      <c r="W15" s="38"/>
+      <c r="X15" s="16">
         <v>0.05</v>
       </c>
-      <c r="X15" s="33"/>
       <c r="Y15" s="33"/>
       <c r="Z15" s="33"/>
       <c r="AA15" s="33"/>
       <c r="AB15" s="33"/>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC15" s="33"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B16" s="23" t="s">
         <v>129</v>
       </c>
@@ -2735,26 +2764,29 @@
       <c r="P16" s="36">
         <v>0.5</v>
       </c>
-      <c r="R16" s="34"/>
-      <c r="S16" s="77">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-      <c r="T16" s="5"/>
-      <c r="U16" s="18" t="s">
+      <c r="R16" s="36">
+        <v>1</v>
+      </c>
+      <c r="S16" s="34"/>
+      <c r="T16" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U16" s="5"/>
+      <c r="V16" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="V16" s="5"/>
-      <c r="W16" s="8">
+      <c r="W16" s="5"/>
+      <c r="X16" s="8">
         <v>0.3</v>
       </c>
-      <c r="X16" s="33"/>
       <c r="Y16" s="33"/>
       <c r="Z16" s="33"/>
       <c r="AA16" s="33"/>
       <c r="AB16" s="33"/>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC16" s="33"/>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B17" s="23" t="s">
         <v>130</v>
       </c>
@@ -2778,26 +2810,29 @@
       <c r="Q17" s="36">
         <v>1</v>
       </c>
-      <c r="R17" s="34"/>
-      <c r="S17" s="77">
+      <c r="R17" s="36">
+        <v>1</v>
+      </c>
+      <c r="S17" s="34"/>
+      <c r="T17" s="77">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="T17" s="5"/>
-      <c r="U17" s="18" t="s">
+      <c r="U17" s="5"/>
+      <c r="V17" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="V17" s="5"/>
-      <c r="W17" s="8">
+      <c r="W17" s="5"/>
+      <c r="X17" s="8">
         <v>3</v>
       </c>
-      <c r="X17" s="33"/>
       <c r="Y17" s="33"/>
       <c r="Z17" s="33"/>
       <c r="AA17" s="33"/>
       <c r="AB17" s="33"/>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC17" s="33"/>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B18" s="23" t="s">
         <v>131</v>
       </c>
@@ -2835,26 +2870,29 @@
       <c r="Q18" s="36">
         <v>1</v>
       </c>
-      <c r="R18" s="34"/>
-      <c r="S18" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T18" s="5"/>
-      <c r="U18" s="18" t="s">
+      <c r="R18" s="36">
+        <v>1</v>
+      </c>
+      <c r="S18" s="34"/>
+      <c r="T18" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U18" s="5"/>
+      <c r="V18" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="V18" s="5"/>
-      <c r="W18" s="39">
+      <c r="W18" s="5"/>
+      <c r="X18" s="39">
         <v>0.25</v>
       </c>
-      <c r="X18" s="33"/>
       <c r="Y18" s="33"/>
       <c r="Z18" s="33"/>
       <c r="AA18" s="33"/>
       <c r="AB18" s="33"/>
-    </row>
-    <row r="19" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AC18" s="33"/>
+    </row>
+    <row r="19" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="23" t="s">
         <v>132</v>
       </c>
@@ -2867,26 +2905,26 @@
         <v>0</v>
       </c>
       <c r="M19" s="36"/>
-      <c r="R19" s="34"/>
-      <c r="S19" s="77">
+      <c r="S19" s="34"/>
+      <c r="T19" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T19" s="15"/>
-      <c r="U19" s="19" t="s">
+      <c r="U19" s="15"/>
+      <c r="V19" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="V19" s="40"/>
-      <c r="W19" s="41">
+      <c r="W19" s="40"/>
+      <c r="X19" s="41">
         <v>0.05</v>
       </c>
-      <c r="X19" s="33"/>
       <c r="Y19" s="33"/>
       <c r="Z19" s="33"/>
       <c r="AA19" s="33"/>
       <c r="AB19" s="33"/>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC19" s="33"/>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B20" s="23" t="s">
         <v>133</v>
       </c>
@@ -2899,19 +2937,19 @@
         <v>0</v>
       </c>
       <c r="M20" s="36"/>
-      <c r="R20" s="34"/>
-      <c r="S20" s="77">
+      <c r="S20" s="34"/>
+      <c r="T20" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T20" s="15"/>
-      <c r="X20" s="33"/>
+      <c r="U20" s="15"/>
       <c r="Y20" s="33"/>
       <c r="Z20" s="33"/>
       <c r="AA20" s="33"/>
       <c r="AB20" s="33"/>
-    </row>
-    <row r="21" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AC20" s="33"/>
+    </row>
+    <row r="21" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="23" t="s">
         <v>134</v>
       </c>
@@ -2924,22 +2962,22 @@
         <v>0</v>
       </c>
       <c r="M21" s="36"/>
-      <c r="R21" s="34"/>
-      <c r="S21" s="77">
+      <c r="S21" s="34"/>
+      <c r="T21" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T21" s="15"/>
       <c r="U21" s="15"/>
-      <c r="V21" s="6"/>
+      <c r="V21" s="15"/>
       <c r="W21" s="6"/>
-      <c r="X21" s="33"/>
+      <c r="X21" s="6"/>
       <c r="Y21" s="33"/>
       <c r="Z21" s="33"/>
       <c r="AA21" s="33"/>
       <c r="AB21" s="33"/>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC21" s="33"/>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B22" s="23" t="s">
         <v>135</v>
       </c>
@@ -2953,30 +2991,30 @@
       <c r="P22" s="36">
         <v>0.5</v>
       </c>
-      <c r="R22" s="34"/>
-      <c r="S22" s="77">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="T22" s="15"/>
-      <c r="U22" s="46" t="s">
+      <c r="S22" s="34"/>
+      <c r="T22" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U22" s="15"/>
+      <c r="V22" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="V22" s="4" t="s">
+      <c r="W22" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="W22" s="4" t="s">
+      <c r="X22" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="X22" s="7" t="s">
+      <c r="Y22" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="Y22" s="33"/>
       <c r="Z22" s="33"/>
       <c r="AA22" s="33"/>
       <c r="AB22" s="33"/>
-    </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC22" s="33"/>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B23" s="23" t="s">
         <v>136</v>
       </c>
@@ -2987,33 +3025,33 @@
       <c r="L23" s="2">
         <v>0</v>
       </c>
-      <c r="R23" s="34"/>
-      <c r="S23" s="77">
+      <c r="S23" s="34"/>
+      <c r="T23" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T23" s="15"/>
-      <c r="U23" s="81">
+      <c r="U23" s="15"/>
+      <c r="V23" s="81">
         <v>0</v>
       </c>
-      <c r="V23" s="6">
-        <f>SUMIF(S$2:S$71,"&gt;=" &amp; U23,C$2:C$71)</f>
+      <c r="W23" s="6">
+        <f t="shared" ref="W23:W31" si="1">SUMIF(T$2:T$71,"&gt;=" &amp; V23,C$2:C$71)</f>
         <v>303</v>
       </c>
-      <c r="W23" s="6">
-        <f>SUMIF(S$2:S$71,"&gt;=" &amp; U23,D$2:D$71)</f>
+      <c r="X23" s="6">
+        <f t="shared" ref="X23:X31" si="2">SUMIF(T$2:T$71,"&gt;=" &amp; V23,D$2:D$71)</f>
         <v>7</v>
       </c>
-      <c r="X23" s="8">
-        <f t="shared" ref="X23:X31" si="1">($W$17 + $W$15*V23+$W$16*W23)*(1+W$18+W$19)</f>
+      <c r="Y23" s="8">
+        <f t="shared" ref="Y23:Y31" si="3">($X$17 + $X$15*W23+$X$16*X23)*(1+X$18+X$19)</f>
         <v>26.324999999999999</v>
       </c>
-      <c r="Y23" s="33"/>
       <c r="Z23" s="33"/>
       <c r="AA23" s="33"/>
       <c r="AB23" s="33"/>
-    </row>
-    <row r="24" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AC23" s="33"/>
+    </row>
+    <row r="24" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="23" t="s">
         <v>137</v>
@@ -3055,33 +3093,36 @@
       <c r="Q24" s="36">
         <v>1</v>
       </c>
-      <c r="R24" s="34"/>
-      <c r="S24" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T24" s="15"/>
-      <c r="U24" s="81">
+      <c r="R24" s="36">
+        <v>1</v>
+      </c>
+      <c r="S24" s="34"/>
+      <c r="T24" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U24" s="15"/>
+      <c r="V24" s="81">
         <v>0.5</v>
       </c>
-      <c r="V24" s="6">
-        <f>SUMIF(S$2:S$71,"&gt;=" &amp; U24,C$2:C$71)</f>
-        <v>251</v>
-      </c>
       <c r="W24" s="6">
-        <f>SUMIF(S$2:S$71,"&gt;=" &amp; U24,D$2:D$71)</f>
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
+      <c r="X24" s="6">
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="X24" s="8">
-        <f t="shared" si="1"/>
-        <v>22.555000000000003</v>
-      </c>
-      <c r="Y24" s="33"/>
+      <c r="Y24" s="8">
+        <f t="shared" si="3"/>
+        <v>22.490000000000002</v>
+      </c>
       <c r="Z24" s="33"/>
       <c r="AA24" s="33"/>
       <c r="AB24" s="33"/>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC24" s="33"/>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B25" s="23" t="s">
         <v>138</v>
       </c>
@@ -3109,33 +3150,36 @@
       <c r="Q25" s="36">
         <v>1</v>
       </c>
-      <c r="R25" s="34"/>
-      <c r="S25" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T25" s="15"/>
-      <c r="U25" s="81">
-        <v>1</v>
-      </c>
-      <c r="V25" s="6">
-        <f>SUMIF(S$2:S$71,"&gt;=" &amp; U25,C$2:C$71)</f>
-        <v>247</v>
+      <c r="R25" s="36">
+        <v>1</v>
+      </c>
+      <c r="S25" s="34"/>
+      <c r="T25" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U25" s="15"/>
+      <c r="V25" s="81">
+        <v>1</v>
       </c>
       <c r="W25" s="6">
-        <f>SUMIF(S$2:S$71,"&gt;=" &amp; U25,D$2:D$71)</f>
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
+      <c r="X25" s="6">
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="X25" s="8">
-        <f t="shared" si="1"/>
-        <v>22.295000000000005</v>
-      </c>
-      <c r="Y25" s="33"/>
+      <c r="Y25" s="8">
+        <f t="shared" si="3"/>
+        <v>22.490000000000002</v>
+      </c>
       <c r="Z25" s="33"/>
       <c r="AA25" s="33"/>
       <c r="AB25" s="33"/>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC25" s="33"/>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B26" s="23" t="s">
         <v>139</v>
       </c>
@@ -3170,33 +3214,36 @@
       <c r="Q26" s="36">
         <v>1</v>
       </c>
-      <c r="R26" s="34"/>
-      <c r="S26" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T26" s="15"/>
-      <c r="U26" s="82">
+      <c r="R26" s="36">
+        <v>1</v>
+      </c>
+      <c r="S26" s="34"/>
+      <c r="T26" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U26" s="15"/>
+      <c r="V26" s="82">
         <v>1.5</v>
       </c>
-      <c r="V26" s="31">
-        <f>SUMIF(S$2:S$71,"&gt;=" &amp; U26,C$2:C$71)</f>
-        <v>241</v>
-      </c>
       <c r="W26" s="31">
-        <f>SUMIF(S$2:S$71,"&gt;=" &amp; U26,D$2:D$71)</f>
+        <f t="shared" si="1"/>
+        <v>198</v>
+      </c>
+      <c r="X26" s="31">
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="X26" s="8">
-        <f t="shared" si="1"/>
-        <v>21.905000000000001</v>
-      </c>
-      <c r="Y26" s="33"/>
+      <c r="Y26" s="8">
+        <f t="shared" si="3"/>
+        <v>19.11</v>
+      </c>
       <c r="Z26" s="33"/>
       <c r="AA26" s="33"/>
       <c r="AB26" s="33"/>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC26" s="33"/>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>117</v>
       </c>
@@ -3240,29 +3287,32 @@
       <c r="Q27" s="35">
         <v>1</v>
       </c>
-      <c r="R27" s="35"/>
-      <c r="S27" s="78">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T27" s="15"/>
-      <c r="U27" s="81">
+      <c r="R27" s="35">
+        <v>1</v>
+      </c>
+      <c r="S27" s="35"/>
+      <c r="T27" s="78">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="V27" s="6">
-        <f>SUMIF(S$2:S$71,"&gt;=" &amp; U27,C$2:C$71)</f>
-        <v>232</v>
+      <c r="U27" s="15"/>
+      <c r="V27" s="81">
+        <v>2</v>
       </c>
       <c r="W27" s="6">
-        <f>SUMIF(S$2:S$71,"&gt;=" &amp; U27,D$2:D$71)</f>
+        <f t="shared" si="1"/>
+        <v>185</v>
+      </c>
+      <c r="X27" s="6">
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="X27" s="8">
-        <f t="shared" si="1"/>
-        <v>21.320000000000004</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="Y27" s="8">
+        <f t="shared" si="3"/>
+        <v>18.265000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B28" s="23" t="s">
         <v>141</v>
       </c>
@@ -3297,29 +3347,29 @@
       <c r="Q28" s="36">
         <v>1</v>
       </c>
-      <c r="R28" s="34"/>
-      <c r="S28" s="77">
-        <f t="shared" si="0"/>
-        <v>2.75</v>
-      </c>
-      <c r="T28" s="15"/>
-      <c r="U28" s="81">
+      <c r="S28" s="34"/>
+      <c r="T28" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U28" s="15"/>
+      <c r="V28" s="81">
         <v>2.5</v>
       </c>
-      <c r="V28" s="6">
-        <f>SUMIF(S$2:S$71,"&gt;=" &amp; U28,C$2:C$71)</f>
-        <v>192</v>
-      </c>
       <c r="W28" s="6">
-        <f>SUMIF(S$2:S$71,"&gt;=" &amp; U28,D$2:D$71)</f>
-        <v>6</v>
-      </c>
-      <c r="X28" s="8">
         <f t="shared" si="1"/>
-        <v>18.720000000000002</v>
-      </c>
-    </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="X28" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Y28" s="8">
+        <f t="shared" si="3"/>
+        <v>4.16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B29" s="23" t="s">
         <v>142</v>
       </c>
@@ -3333,29 +3383,29 @@
       <c r="L29" s="2">
         <v>0.7</v>
       </c>
-      <c r="R29" s="34"/>
-      <c r="S29" s="77">
+      <c r="S29" s="34"/>
+      <c r="T29" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T29" s="15"/>
-      <c r="U29" s="81">
+      <c r="U29" s="15"/>
+      <c r="V29" s="81">
         <v>3</v>
       </c>
-      <c r="V29" s="6">
-        <f>SUMIF(S$2:S$71,"&gt;=" &amp; U29,C$2:C$71)</f>
-        <v>166</v>
-      </c>
       <c r="W29" s="6">
-        <f>SUMIF(S$2:S$71,"&gt;=" &amp; U29,D$2:D$71)</f>
-        <v>6</v>
-      </c>
-      <c r="X29" s="8">
         <f t="shared" si="1"/>
-        <v>17.03</v>
-      </c>
-    </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="X29" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Y29" s="8">
+        <f t="shared" si="3"/>
+        <v>4.16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B30" s="23" t="s">
         <v>143</v>
       </c>
@@ -3388,29 +3438,29 @@
       <c r="Q30" s="36">
         <v>1</v>
       </c>
-      <c r="R30" s="34"/>
-      <c r="S30" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T30" s="15"/>
-      <c r="U30" s="81">
+      <c r="S30" s="34"/>
+      <c r="T30" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U30" s="15"/>
+      <c r="V30" s="81">
         <v>3.5</v>
       </c>
-      <c r="V30" s="6">
-        <f>SUMIF(S$2:S$71,"&gt;=" &amp; U30,C$2:C$71)</f>
+      <c r="W30" s="6">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="W30" s="6">
-        <f>SUMIF(S$2:S$71,"&gt;=" &amp; U30,D$2:D$71)</f>
+      <c r="X30" s="6">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X30" s="8">
-        <f t="shared" si="1"/>
+      <c r="Y30" s="8">
+        <f t="shared" si="3"/>
         <v>3.9000000000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="23" t="s">
         <v>144</v>
       </c>
@@ -3448,29 +3498,32 @@
       <c r="Q31" s="36">
         <v>1</v>
       </c>
-      <c r="R31" s="34"/>
-      <c r="S31" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T31" s="15"/>
-      <c r="U31" s="83">
+      <c r="R31" s="36">
+        <v>1</v>
+      </c>
+      <c r="S31" s="34"/>
+      <c r="T31" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U31" s="15"/>
+      <c r="V31" s="83">
         <v>4</v>
       </c>
-      <c r="V31" s="47">
-        <f>SUMIF(S$2:S$71,"&gt;=" &amp; U31,C$2:C$71)</f>
+      <c r="W31" s="47">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="W31" s="47">
-        <f>SUMIF(S$2:S$71,"&gt;=" &amp; U31,D$2:D$71)</f>
+      <c r="X31" s="47">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X31" s="9">
-        <f t="shared" si="1"/>
+      <c r="Y31" s="9">
+        <f t="shared" si="3"/>
         <v>3.9000000000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="23" t="s">
         <v>145</v>
@@ -3498,17 +3551,18 @@
       <c r="Q32" s="36">
         <v>1</v>
       </c>
-      <c r="R32" s="34"/>
-      <c r="S32" s="77">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-      <c r="T32" s="15"/>
-      <c r="U32" s="3"/>
-      <c r="V32"/>
+      <c r="R32" s="36"/>
+      <c r="S32" s="34"/>
+      <c r="T32" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U32" s="15"/>
+      <c r="V32" s="3"/>
       <c r="W32"/>
-    </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="X32"/>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B33" s="23" t="s">
         <v>146</v>
       </c>
@@ -3546,14 +3600,17 @@
       <c r="Q33" s="36">
         <v>1</v>
       </c>
-      <c r="R33" s="34"/>
-      <c r="S33" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T33" s="15"/>
-    </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="R33" s="36">
+        <v>1</v>
+      </c>
+      <c r="S33" s="34"/>
+      <c r="T33" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U33" s="15"/>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B34" s="23" t="s">
         <v>147</v>
       </c>
@@ -3579,14 +3636,17 @@
       <c r="Q34" s="36">
         <v>1</v>
       </c>
-      <c r="R34" s="34"/>
-      <c r="S34" s="77">
+      <c r="R34" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="S34" s="34"/>
+      <c r="T34" s="77">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="T34" s="15"/>
-    </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U34" s="15"/>
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B35" s="23" t="s">
         <v>148</v>
       </c>
@@ -3621,15 +3681,18 @@
       <c r="Q35" s="36">
         <v>1</v>
       </c>
-      <c r="R35" s="34"/>
-      <c r="S35" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T35" s="15"/>
-      <c r="U35" s="84"/>
-    </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="R35" s="36">
+        <v>1</v>
+      </c>
+      <c r="S35" s="34"/>
+      <c r="T35" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U35" s="15"/>
+      <c r="V35" s="84"/>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B36" s="23" t="s">
         <v>149</v>
       </c>
@@ -3664,15 +3727,18 @@
       <c r="Q36" s="36">
         <v>1</v>
       </c>
-      <c r="R36" s="34"/>
-      <c r="S36" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T36" s="15"/>
-      <c r="U36" s="84"/>
-    </row>
-    <row r="37" spans="1:28" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R36" s="36">
+        <v>1</v>
+      </c>
+      <c r="S36" s="34"/>
+      <c r="T36" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U36" s="15"/>
+      <c r="V36" s="84"/>
+    </row>
+    <row r="37" spans="1:29" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="23" t="s">
         <v>150</v>
@@ -3710,34 +3776,38 @@
       <c r="Q37" s="36">
         <v>1</v>
       </c>
-      <c r="R37" s="34"/>
-      <c r="S37" s="77">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="T37" s="15"/>
-      <c r="U37" s="84"/>
-    </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="R37" s="36"/>
+      <c r="S37" s="34"/>
+      <c r="T37" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U37" s="15"/>
+      <c r="V37" s="84"/>
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B38" s="23" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C38" s="14">
         <v>4</v>
       </c>
       <c r="I38" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="R38" s="34"/>
-      <c r="S38" s="77">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T38" s="15"/>
-      <c r="U38" s="84"/>
-      <c r="X38" s="6"/>
-    </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+      <c r="R38" s="36">
+        <v>1</v>
+      </c>
+      <c r="S38" s="34"/>
+      <c r="T38" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U38" s="15"/>
+      <c r="V38" s="84"/>
+      <c r="Y38" s="6"/>
+    </row>
+    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
         <v>116</v>
       </c>
@@ -3781,14 +3851,17 @@
       <c r="Q39" s="35">
         <v>1</v>
       </c>
-      <c r="R39" s="35"/>
-      <c r="S39" s="78">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T39" s="15"/>
-    </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="R39" s="35">
+        <v>1</v>
+      </c>
+      <c r="S39" s="35"/>
+      <c r="T39" s="78">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U39" s="15"/>
+    </row>
+    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A40" s="30"/>
       <c r="B40" s="31" t="s">
         <v>152</v>
@@ -3827,16 +3900,19 @@
       <c r="Q40" s="36">
         <v>1</v>
       </c>
-      <c r="R40" s="36"/>
-      <c r="S40" s="77">
-        <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-      <c r="T40" s="15"/>
+      <c r="R40" s="36">
+        <v>1</v>
+      </c>
+      <c r="S40" s="36"/>
+      <c r="T40" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="U40" s="15"/>
-      <c r="V40" s="6"/>
-    </row>
-    <row r="41" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="V40" s="15"/>
+      <c r="W40" s="6"/>
+    </row>
+    <row r="41" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="30"/>
       <c r="B41" s="31" t="s">
         <v>153</v>
@@ -3878,21 +3954,24 @@
       <c r="Q41" s="36">
         <v>1</v>
       </c>
-      <c r="R41" s="36"/>
-      <c r="S41" s="77">
-        <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-      <c r="T41" s="15"/>
-      <c r="U41" s="3"/>
-      <c r="V41"/>
+      <c r="R41" s="36">
+        <v>1</v>
+      </c>
+      <c r="S41" s="36"/>
+      <c r="T41" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U41" s="15"/>
+      <c r="V41" s="3"/>
       <c r="W41"/>
-      <c r="Y41"/>
+      <c r="X41"/>
       <c r="Z41"/>
       <c r="AA41"/>
       <c r="AB41"/>
-    </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC41"/>
+    </row>
+    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A42" s="30"/>
       <c r="B42" s="31" t="s">
         <v>154</v>
@@ -3912,18 +3991,18 @@
       <c r="Q42" s="36">
         <v>1</v>
       </c>
-      <c r="R42" s="36"/>
-      <c r="S42" s="77">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="T42" s="15"/>
-      <c r="Y42" s="6"/>
+      <c r="S42" s="36"/>
+      <c r="T42" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U42" s="15"/>
       <c r="Z42" s="6"/>
       <c r="AA42" s="6"/>
       <c r="AB42" s="6"/>
-    </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC42" s="6"/>
+    </row>
+    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A43" s="30"/>
       <c r="B43" s="31" t="s">
         <v>155</v>
@@ -3962,15 +4041,18 @@
       <c r="Q43" s="36">
         <v>1</v>
       </c>
-      <c r="R43" s="36"/>
-      <c r="S43" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T43" s="15"/>
-      <c r="X43" s="6"/>
-    </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="R43" s="36">
+        <v>1</v>
+      </c>
+      <c r="S43" s="36"/>
+      <c r="T43" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U43" s="15"/>
+      <c r="Y43" s="6"/>
+    </row>
+    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A44" s="30"/>
       <c r="B44" s="31" t="s">
         <v>156</v>
@@ -4006,16 +4088,19 @@
       <c r="Q44" s="36">
         <v>1</v>
       </c>
-      <c r="R44" s="36"/>
-      <c r="S44" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T44" s="15"/>
+      <c r="R44" s="36">
+        <v>1</v>
+      </c>
+      <c r="S44" s="36"/>
+      <c r="T44" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="U44" s="15"/>
-      <c r="V44" s="6"/>
-    </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="V44" s="15"/>
+      <c r="W44" s="6"/>
+    </row>
+    <row r="45" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A45" s="30"/>
       <c r="B45" s="31" t="s">
         <v>157</v>
@@ -4051,15 +4136,18 @@
       <c r="Q45" s="36">
         <v>1</v>
       </c>
-      <c r="R45" s="36"/>
-      <c r="S45" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T45" s="15"/>
-      <c r="W45" s="6"/>
-    </row>
-    <row r="46" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R45" s="36">
+        <v>1</v>
+      </c>
+      <c r="S45" s="36"/>
+      <c r="T45" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U45" s="15"/>
+      <c r="X45" s="6"/>
+    </row>
+    <row r="46" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="30"/>
       <c r="B46" s="31" t="s">
         <v>158</v>
@@ -4101,22 +4189,25 @@
       <c r="Q46" s="36">
         <v>1</v>
       </c>
-      <c r="R46" s="36"/>
-      <c r="S46" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T46" s="15"/>
-      <c r="U46" s="3"/>
-      <c r="V46"/>
+      <c r="R46" s="36">
+        <v>1</v>
+      </c>
+      <c r="S46" s="36"/>
+      <c r="T46" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U46" s="15"/>
+      <c r="V46" s="3"/>
       <c r="W46"/>
       <c r="X46"/>
       <c r="Y46"/>
       <c r="Z46"/>
       <c r="AA46"/>
       <c r="AB46"/>
-    </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC46"/>
+    </row>
+    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A47" s="30"/>
       <c r="B47" s="31" t="s">
         <v>159</v>
@@ -4153,14 +4244,17 @@
       <c r="Q47" s="36">
         <v>1</v>
       </c>
-      <c r="R47" s="36"/>
-      <c r="S47" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T47" s="15"/>
-    </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="R47" s="36">
+        <v>0.75</v>
+      </c>
+      <c r="S47" s="36"/>
+      <c r="T47" s="77">
+        <f t="shared" si="0"/>
+        <v>1.75</v>
+      </c>
+      <c r="U47" s="15"/>
+    </row>
+    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B48" s="23" t="s">
         <v>160</v>
       </c>
@@ -4198,14 +4292,17 @@
       <c r="Q48" s="36">
         <v>1</v>
       </c>
-      <c r="R48" s="34"/>
-      <c r="S48" s="77">
-        <f t="shared" si="0"/>
-        <v>2.25</v>
-      </c>
-      <c r="T48" s="15"/>
-    </row>
-    <row r="49" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R48" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="S48" s="34"/>
+      <c r="T48" s="77">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="U48" s="15"/>
+    </row>
+    <row r="49" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
         <v>115</v>
       </c>
@@ -4248,19 +4345,20 @@
         <v>1</v>
       </c>
       <c r="R49" s="35"/>
-      <c r="S49" s="78">
-        <f t="shared" si="0"/>
-        <v>2.25</v>
-      </c>
-      <c r="T49" s="15"/>
+      <c r="S49" s="35"/>
+      <c r="T49" s="78">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="U49" s="15"/>
-      <c r="X49"/>
+      <c r="V49" s="15"/>
       <c r="Y49"/>
       <c r="Z49"/>
       <c r="AA49"/>
       <c r="AB49"/>
-    </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC49"/>
+    </row>
+    <row r="50" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B50" s="23" t="s">
         <v>162</v>
       </c>
@@ -4298,18 +4396,21 @@
       <c r="Q50" s="36">
         <v>1</v>
       </c>
-      <c r="R50" s="34"/>
-      <c r="S50" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T50" s="15"/>
-      <c r="Y50" s="33"/>
-      <c r="Z50" s="6"/>
+      <c r="R50" s="36">
+        <v>1</v>
+      </c>
+      <c r="S50" s="34"/>
+      <c r="T50" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U50" s="15"/>
+      <c r="Z50" s="33"/>
       <c r="AA50" s="6"/>
       <c r="AB50" s="6"/>
-    </row>
-    <row r="51" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AC50" s="6"/>
+    </row>
+    <row r="51" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="10"/>
       <c r="B51" s="23" t="s">
         <v>163</v>
@@ -4351,22 +4452,25 @@
       <c r="Q51" s="36">
         <v>1</v>
       </c>
-      <c r="R51" s="34"/>
-      <c r="S51" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T51" s="15"/>
-      <c r="U51" s="3"/>
-      <c r="V51"/>
+      <c r="R51" s="36">
+        <v>1</v>
+      </c>
+      <c r="S51" s="34"/>
+      <c r="T51" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U51" s="15"/>
+      <c r="V51" s="3"/>
       <c r="W51"/>
       <c r="X51"/>
-      <c r="Y51" s="33"/>
-      <c r="Z51"/>
+      <c r="Y51"/>
+      <c r="Z51" s="33"/>
       <c r="AA51"/>
       <c r="AB51"/>
-    </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC51"/>
+    </row>
+    <row r="52" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B52" s="23" t="s">
         <v>164</v>
       </c>
@@ -4380,15 +4484,15 @@
       <c r="N52" s="36">
         <v>0.5</v>
       </c>
-      <c r="R52" s="34"/>
-      <c r="S52" s="77">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="T52" s="15"/>
-      <c r="Y52" s="33"/>
-    </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="S52" s="34"/>
+      <c r="T52" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U52" s="15"/>
+      <c r="Z52" s="33"/>
+    </row>
+    <row r="53" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B53" s="23" t="s">
         <v>165</v>
       </c>
@@ -4399,18 +4503,18 @@
       <c r="L53" s="2">
         <v>0</v>
       </c>
-      <c r="R53" s="34"/>
-      <c r="S53" s="77">
+      <c r="S53" s="34"/>
+      <c r="T53" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T53" s="15"/>
-      <c r="Y53" s="33"/>
-    </row>
-    <row r="54" spans="1:28" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="U53" s="15"/>
+      <c r="Z53" s="33"/>
+    </row>
+    <row r="54" spans="1:29" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="10"/>
       <c r="B54" s="23" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C54" s="14">
         <v>3</v>
@@ -4423,7 +4527,7 @@
       <c r="G54" s="14"/>
       <c r="H54" s="14"/>
       <c r="I54" s="22" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="J54" s="36"/>
       <c r="K54" s="34"/>
@@ -4433,15 +4537,16 @@
       <c r="O54" s="36"/>
       <c r="P54" s="36"/>
       <c r="Q54" s="36"/>
-      <c r="R54" s="34"/>
-      <c r="S54" s="77">
+      <c r="R54" s="36"/>
+      <c r="S54" s="34"/>
+      <c r="T54" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T54" s="15"/>
-      <c r="U54" s="3"/>
-    </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U54" s="15"/>
+      <c r="V54" s="3"/>
+    </row>
+    <row r="55" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B55" s="23" t="s">
         <v>166</v>
       </c>
@@ -4458,16 +4563,19 @@
       <c r="L55" s="2">
         <v>0.7</v>
       </c>
-      <c r="R55" s="34"/>
-      <c r="S55" s="77">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T55" s="15"/>
-      <c r="W55" s="6"/>
-      <c r="Y55" s="33"/>
-    </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="R55" s="36">
+        <v>1</v>
+      </c>
+      <c r="S55" s="34"/>
+      <c r="T55" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U55" s="15"/>
+      <c r="X55" s="6"/>
+      <c r="Z55" s="33"/>
+    </row>
+    <row r="56" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B56" s="23" t="s">
         <v>167</v>
       </c>
@@ -4505,15 +4613,18 @@
       <c r="Q56" s="36">
         <v>1</v>
       </c>
-      <c r="R56" s="34"/>
-      <c r="S56" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T56" s="15"/>
-      <c r="Y56" s="33"/>
-    </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="R56" s="36">
+        <v>1</v>
+      </c>
+      <c r="S56" s="34"/>
+      <c r="T56" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U56" s="15"/>
+      <c r="Z56" s="33"/>
+    </row>
+    <row r="57" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
         <v>114</v>
       </c>
@@ -4554,15 +4665,16 @@
         <v>1</v>
       </c>
       <c r="R57" s="35"/>
-      <c r="S57" s="78">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T57" s="15"/>
-      <c r="X57" s="6"/>
-      <c r="Y57" s="33"/>
-    </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="S57" s="35"/>
+      <c r="T57" s="78">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U57" s="15"/>
+      <c r="Y57" s="6"/>
+      <c r="Z57" s="33"/>
+    </row>
+    <row r="58" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B58" s="23" t="s">
         <v>169</v>
       </c>
@@ -4600,15 +4712,18 @@
       <c r="Q58" s="36">
         <v>1</v>
       </c>
-      <c r="R58" s="34"/>
-      <c r="S58" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T58" s="15"/>
-      <c r="Y58" s="33"/>
-    </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="R58" s="36">
+        <v>1</v>
+      </c>
+      <c r="S58" s="34"/>
+      <c r="T58" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U58" s="15"/>
+      <c r="Z58" s="33"/>
+    </row>
+    <row r="59" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B59" s="23" t="s">
         <v>170</v>
       </c>
@@ -4646,18 +4761,21 @@
       <c r="Q59" s="36">
         <v>1</v>
       </c>
-      <c r="R59" s="34"/>
-      <c r="S59" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T59" s="15"/>
-      <c r="Y59" s="33"/>
-      <c r="Z59" s="6"/>
+      <c r="R59" s="36">
+        <v>1</v>
+      </c>
+      <c r="S59" s="34"/>
+      <c r="T59" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U59" s="15"/>
+      <c r="Z59" s="33"/>
       <c r="AA59" s="6"/>
       <c r="AB59" s="6"/>
-    </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC59" s="6"/>
+    </row>
+    <row r="60" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B60" s="23" t="s">
         <v>171</v>
       </c>
@@ -4668,15 +4786,15 @@
       <c r="L60" s="2">
         <v>0</v>
       </c>
-      <c r="R60" s="34"/>
-      <c r="S60" s="77">
+      <c r="S60" s="34"/>
+      <c r="T60" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T60" s="15"/>
-      <c r="Y60" s="33"/>
-    </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U60" s="15"/>
+      <c r="Z60" s="33"/>
+    </row>
+    <row r="61" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
         <v>113</v>
       </c>
@@ -4711,15 +4829,16 @@
       <c r="P61" s="35"/>
       <c r="Q61" s="35"/>
       <c r="R61" s="35"/>
-      <c r="S61" s="78">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="T61" s="15"/>
-      <c r="X61" s="6"/>
-      <c r="Y61" s="33"/>
-    </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="S61" s="35"/>
+      <c r="T61" s="78">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U61" s="15"/>
+      <c r="Y61" s="6"/>
+      <c r="Z61" s="33"/>
+    </row>
+    <row r="62" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B62" s="23" t="s">
         <v>173</v>
       </c>
@@ -4742,15 +4861,15 @@
       <c r="O62" s="36">
         <v>1</v>
       </c>
-      <c r="R62" s="34"/>
-      <c r="S62" s="77">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="T62" s="15"/>
-      <c r="Y62" s="33"/>
-    </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="S62" s="34"/>
+      <c r="T62" s="77">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U62" s="15"/>
+      <c r="Z62" s="33"/>
+    </row>
+    <row r="63" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A63" s="11" t="s">
         <v>74</v>
       </c>
@@ -4786,14 +4905,17 @@
       <c r="Q63" s="35">
         <v>1</v>
       </c>
-      <c r="R63" s="35"/>
-      <c r="S63" s="78">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T63" s="15"/>
-    </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="R63" s="35">
+        <v>1</v>
+      </c>
+      <c r="S63" s="35"/>
+      <c r="T63" s="78">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U63" s="15"/>
+    </row>
+    <row r="64" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A64" s="30"/>
       <c r="B64" s="31" t="s">
         <v>82</v>
@@ -4818,14 +4940,17 @@
       <c r="Q64" s="36">
         <v>1</v>
       </c>
-      <c r="R64" s="36"/>
-      <c r="S64" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T64" s="15"/>
-    </row>
-    <row r="65" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R64" s="36">
+        <v>1</v>
+      </c>
+      <c r="S64" s="36"/>
+      <c r="T64" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U64" s="15"/>
+    </row>
+    <row r="65" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="10"/>
       <c r="B65" s="23" t="s">
         <v>93</v>
@@ -4841,7 +4966,7 @@
       <c r="G65" s="14"/>
       <c r="H65" s="14"/>
       <c r="I65" s="22" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J65" s="36"/>
       <c r="K65" s="2">
@@ -4855,22 +4980,23 @@
       <c r="O65" s="36"/>
       <c r="P65" s="36"/>
       <c r="Q65" s="36"/>
-      <c r="R65" s="34"/>
-      <c r="S65" s="77">
+      <c r="R65" s="36"/>
+      <c r="S65" s="34"/>
+      <c r="T65" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T65" s="15"/>
-      <c r="U65" s="3"/>
-      <c r="V65"/>
+      <c r="U65" s="15"/>
+      <c r="V65" s="3"/>
       <c r="W65"/>
       <c r="X65"/>
       <c r="Y65"/>
       <c r="Z65"/>
       <c r="AA65"/>
       <c r="AB65"/>
-    </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC65"/>
+    </row>
+    <row r="66" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B66" s="23" t="s">
         <v>94</v>
       </c>
@@ -4896,16 +5022,19 @@
       <c r="Q66" s="36">
         <v>1</v>
       </c>
-      <c r="R66" s="34"/>
-      <c r="S66" s="77">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="T66" s="15"/>
-      <c r="V66" s="33"/>
-      <c r="X66" s="6"/>
-    </row>
-    <row r="67" spans="1:28" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R66" s="36">
+        <v>1</v>
+      </c>
+      <c r="S66" s="34"/>
+      <c r="T66" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U66" s="15"/>
+      <c r="W66" s="33"/>
+      <c r="Y66" s="6"/>
+    </row>
+    <row r="67" spans="1:29" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="10"/>
       <c r="B67" s="23" t="s">
         <v>180</v>
@@ -4929,18 +5058,19 @@
       <c r="Q67" s="36">
         <v>1</v>
       </c>
-      <c r="R67" s="34">
-        <v>1</v>
-      </c>
-      <c r="S67" s="77">
-        <f t="shared" si="0"/>
+      <c r="R67" s="36"/>
+      <c r="S67" s="34">
+        <v>1</v>
+      </c>
+      <c r="T67" s="77">
+        <f t="shared" ref="T67:T70" si="4">SUM(Q67:S67)</f>
         <v>2</v>
       </c>
-      <c r="T67" s="15"/>
-      <c r="U67" s="3"/>
-      <c r="X67" s="6"/>
-    </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U67" s="15"/>
+      <c r="V67" s="3"/>
+      <c r="Y67" s="6"/>
+    </row>
+    <row r="68" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B68" s="23" t="s">
         <v>95</v>
       </c>
@@ -4968,18 +5098,21 @@
       <c r="Q68" s="36">
         <v>1</v>
       </c>
-      <c r="R68" s="34"/>
-      <c r="S68" s="77">
-        <f t="shared" ref="S68:S70" si="2">SUM(N68:R68)</f>
-        <v>3</v>
-      </c>
-      <c r="T68" s="15"/>
-      <c r="Y68" s="6"/>
+      <c r="R68" s="36">
+        <v>1</v>
+      </c>
+      <c r="S68" s="34"/>
+      <c r="T68" s="77">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="U68" s="15"/>
       <c r="Z68" s="6"/>
       <c r="AA68" s="6"/>
       <c r="AB68" s="6"/>
-    </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC68" s="6"/>
+    </row>
+    <row r="69" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B69" s="23" t="s">
         <v>96</v>
       </c>
@@ -5005,14 +5138,17 @@
       <c r="Q69" s="36">
         <v>1</v>
       </c>
-      <c r="R69" s="34"/>
-      <c r="S69" s="77">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="T69" s="15"/>
-    </row>
-    <row r="70" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R69" s="36">
+        <v>1</v>
+      </c>
+      <c r="S69" s="34"/>
+      <c r="T69" s="77">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="U69" s="15"/>
+    </row>
+    <row r="70" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="10"/>
       <c r="B70" s="24" t="s">
         <v>97</v>
@@ -5041,27 +5177,30 @@
       <c r="P70" s="37"/>
       <c r="Q70" s="37"/>
       <c r="R70" s="37">
+        <v>1</v>
+      </c>
+      <c r="S70" s="37">
         <v>2</v>
       </c>
-      <c r="S70" s="79">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="T70" s="15"/>
-      <c r="U70" s="3"/>
-      <c r="V70"/>
+      <c r="T70" s="79">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="U70" s="15"/>
+      <c r="V70" s="3"/>
       <c r="W70"/>
       <c r="X70"/>
       <c r="Y70"/>
       <c r="Z70"/>
       <c r="AA70"/>
       <c r="AB70"/>
-    </row>
-    <row r="71" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AC70"/>
+    </row>
+    <row r="71" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="11"/>
-      <c r="T71" s="15"/>
-    </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U71" s="15"/>
+    </row>
+    <row r="72" spans="1:29" x14ac:dyDescent="0.3">
       <c r="I72" s="64" t="s">
         <v>98</v>
       </c>
@@ -5069,27 +5208,22 @@
       <c r="K72" s="65"/>
       <c r="L72" s="65"/>
       <c r="M72" s="65"/>
-      <c r="N72" s="65">
-        <f t="array" ref="N72">SUM($C2:$C70*(N2:N70&gt;=0.9)*($S2:$S70&gt;=$U$12))</f>
-        <v>191</v>
-      </c>
-      <c r="O72" s="65">
-        <f t="array" ref="O72">SUM($C2:$C70*(O2:O70&gt;=0.9)*($S2:$S70&gt;=$U$12))</f>
-        <v>14</v>
-      </c>
-      <c r="P72" s="65">
-        <f t="array" ref="P72">SUM($C2:$C70*(P2:P70&gt;=0.9)*($S2:$S70&gt;=$U$12))</f>
-        <v>187</v>
-      </c>
+      <c r="N72" s="65"/>
+      <c r="O72" s="65"/>
+      <c r="P72" s="65"/>
       <c r="Q72" s="65">
-        <f t="array" ref="Q72">SUM($C2:$C70*(Q2:Q70&gt;=0.9)*($S2:$S70&gt;=$U$12))</f>
-        <v>227</v>
-      </c>
-      <c r="R72" s="66"/>
-      <c r="T72" s="15"/>
-      <c r="W72" s="33"/>
-    </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.3">
+        <f t="array" ref="Q72">SUM($C2:$C70*(Q2:Q70&gt;=0.9)*($T2:$T70&gt;=$V$12))</f>
+        <v>194</v>
+      </c>
+      <c r="R72" s="65">
+        <f t="array" ref="R72">SUM($C2:$C70*(R2:R70&gt;=0.9)*($T2:$T70&gt;=$V$12))</f>
+        <v>184</v>
+      </c>
+      <c r="S72" s="66"/>
+      <c r="U72" s="15"/>
+      <c r="X72" s="33"/>
+    </row>
+    <row r="73" spans="1:29" x14ac:dyDescent="0.3">
       <c r="I73" s="67" t="s">
         <v>100</v>
       </c>
@@ -5097,30 +5231,25 @@
       <c r="K73" s="68"/>
       <c r="L73" s="68"/>
       <c r="M73" s="68"/>
-      <c r="N73" s="68">
-        <f t="array" ref="N73">SUM($C2:$C70*N2:N70*($S2:$S70&gt;=$U$12))</f>
-        <v>201</v>
-      </c>
-      <c r="O73" s="68">
-        <f t="array" ref="O73">SUM($C2:$C70*O2:O70*($S2:$S70&gt;=$U$12))</f>
-        <v>14</v>
-      </c>
-      <c r="P73" s="68">
-        <f t="array" ref="P73">SUM($C2:$C70*P2:P70*($S2:$S70&gt;=$U$12))</f>
-        <v>210.5</v>
-      </c>
+      <c r="N73" s="68"/>
+      <c r="O73" s="68"/>
+      <c r="P73" s="68"/>
       <c r="Q73" s="68">
-        <f t="array" ref="Q73">SUM($C2:$C70*Q2:Q70*($S2:$S70&gt;=$U$12))</f>
-        <v>227</v>
-      </c>
-      <c r="R73" s="69"/>
-      <c r="T73" s="15"/>
-      <c r="Y73" s="6"/>
+        <f t="array" ref="Q73">SUM($C2:$C70*Q2:Q70*($T2:$T70&gt;=$V$12))</f>
+        <v>194</v>
+      </c>
+      <c r="R73" s="68">
+        <f t="array" ref="R73">SUM($C2:$C70*R2:R70*($T2:$T70&gt;=$V$12))</f>
+        <v>192</v>
+      </c>
+      <c r="S73" s="69"/>
+      <c r="U73" s="15"/>
       <c r="Z73" s="6"/>
       <c r="AA73" s="6"/>
       <c r="AB73" s="6"/>
-    </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC73" s="6"/>
+    </row>
+    <row r="74" spans="1:29" x14ac:dyDescent="0.3">
       <c r="I74" s="67" t="s">
         <v>99</v>
       </c>
@@ -5128,26 +5257,21 @@
       <c r="K74" s="68"/>
       <c r="L74" s="68"/>
       <c r="M74" s="68"/>
-      <c r="N74" s="68">
-        <f t="array" ref="N74">SUM($C$2:$C$70*(N$2:N$70&gt;=0.1)*($S$2:$S$70&gt;=$U$12))</f>
-        <v>211</v>
-      </c>
-      <c r="O74" s="68">
-        <f t="array" ref="O74">SUM($C$2:$C$70*(O$2:O$70&gt;=0.1)*($S$2:$S$70&gt;=$U$12))</f>
-        <v>14</v>
-      </c>
-      <c r="P74" s="68">
-        <f t="array" ref="P74">SUM($C$2:$C$70*(P$2:P$70&gt;=0.1)*($S$2:$S$70&gt;=$U$12))</f>
-        <v>224</v>
-      </c>
+      <c r="N74" s="68"/>
+      <c r="O74" s="68"/>
+      <c r="P74" s="68"/>
       <c r="Q74" s="68">
-        <f t="array" ref="Q74">SUM($C$2:$C$70*(Q$2:Q$70&gt;=0.1)*($S$2:$S$70&gt;=$U$12))</f>
-        <v>227</v>
-      </c>
-      <c r="R74" s="69"/>
-      <c r="T74" s="15"/>
-    </row>
-    <row r="75" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="array" ref="Q74">SUM($C$2:$C$70*(Q$2:Q$70&gt;=0.1)*($T$2:$T$70&gt;=$V$12))</f>
+        <v>194</v>
+      </c>
+      <c r="R74" s="68">
+        <f t="array" ref="R74">SUM($C$2:$C$70*(R$2:R$70&gt;=0.1)*($T$2:$T$70&gt;=$V$12))</f>
+        <v>197</v>
+      </c>
+      <c r="S74" s="69"/>
+      <c r="U74" s="15"/>
+    </row>
+    <row r="75" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="10"/>
       <c r="B75" s="23"/>
       <c r="C75" s="14"/>
@@ -5163,35 +5287,30 @@
       <c r="K75" s="68"/>
       <c r="L75" s="68"/>
       <c r="M75" s="68"/>
-      <c r="N75" s="68">
-        <f t="shared" ref="N75:Q75" si="3">LOOKUP($U$12,$U23:$U31,$V23:$V31)</f>
-        <v>241</v>
-      </c>
-      <c r="O75" s="68">
-        <f t="shared" si="3"/>
-        <v>241</v>
-      </c>
-      <c r="P75" s="68">
-        <f t="shared" si="3"/>
-        <v>241</v>
-      </c>
+      <c r="N75" s="68"/>
+      <c r="O75" s="68"/>
+      <c r="P75" s="68"/>
       <c r="Q75" s="68">
-        <f t="shared" si="3"/>
-        <v>241</v>
-      </c>
-      <c r="R75" s="69"/>
-      <c r="S75" s="3"/>
-      <c r="T75" s="15"/>
-      <c r="U75" s="3"/>
-      <c r="V75"/>
+        <f t="shared" ref="Q75:R75" si="5">LOOKUP($V$12,$V23:$V31,$W23:$W31)</f>
+        <v>198</v>
+      </c>
+      <c r="R75" s="68">
+        <f t="shared" si="5"/>
+        <v>198</v>
+      </c>
+      <c r="S75" s="69"/>
+      <c r="T75" s="3"/>
+      <c r="U75" s="15"/>
+      <c r="V75" s="3"/>
       <c r="W75"/>
       <c r="X75"/>
       <c r="Y75"/>
       <c r="Z75"/>
       <c r="AA75"/>
       <c r="AB75"/>
-    </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC75"/>
+    </row>
+    <row r="76" spans="1:29" x14ac:dyDescent="0.3">
       <c r="I76" s="67" t="s">
         <v>102</v>
       </c>
@@ -5199,30 +5318,25 @@
       <c r="K76" s="70"/>
       <c r="L76" s="70"/>
       <c r="M76" s="70"/>
-      <c r="N76" s="70">
-        <f t="shared" ref="N76:Q76" si="4">N73/N75</f>
-        <v>0.8340248962655602</v>
-      </c>
-      <c r="O76" s="70">
-        <f t="shared" si="4"/>
-        <v>5.8091286307053944E-2</v>
-      </c>
-      <c r="P76" s="70">
-        <f t="shared" si="4"/>
-        <v>0.87344398340248963</v>
-      </c>
+      <c r="N76" s="70"/>
+      <c r="O76" s="70"/>
+      <c r="P76" s="70"/>
       <c r="Q76" s="70">
-        <f t="shared" si="4"/>
-        <v>0.94190871369294604</v>
-      </c>
-      <c r="R76" s="71"/>
-      <c r="T76" s="15"/>
-      <c r="Y76" s="6"/>
+        <f t="shared" ref="Q76:R76" si="6">Q73/Q75</f>
+        <v>0.97979797979797978</v>
+      </c>
+      <c r="R76" s="70">
+        <f t="shared" si="6"/>
+        <v>0.96969696969696972</v>
+      </c>
+      <c r="S76" s="71"/>
+      <c r="U76" s="15"/>
       <c r="Z76" s="6"/>
       <c r="AA76" s="6"/>
       <c r="AB76" s="6"/>
-    </row>
-    <row r="77" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AC76" s="6"/>
+    </row>
+    <row r="77" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C77" s="33"/>
       <c r="I77" s="72" t="s">
         <v>80</v>
@@ -5231,99 +5345,94 @@
       <c r="K77" s="73"/>
       <c r="L77" s="73"/>
       <c r="M77" s="73"/>
-      <c r="N77" s="73">
-        <f t="array" ref="N77">SUM($C2:$C70*N2:N70*($S2:$S70&lt;$U$12))</f>
-        <v>1.5</v>
-      </c>
-      <c r="O77" s="73">
-        <f t="array" ref="O77">SUM($C2:$C70*O2:O70*($S2:$S70&lt;$U$12))</f>
-        <v>0</v>
-      </c>
-      <c r="P77" s="73">
-        <f t="array" ref="P77">SUM($C2:$C70*P2:P70*($S2:$S70&lt;$U$12))</f>
-        <v>0.5</v>
-      </c>
+      <c r="N77" s="73"/>
+      <c r="O77" s="73"/>
+      <c r="P77" s="73"/>
       <c r="Q77" s="73">
-        <f t="array" ref="Q77">SUM($C2:$C70*Q2:Q70*($S2:$S70&lt;$U$12))</f>
+        <f>Q75-Q73</f>
+        <v>4</v>
+      </c>
+      <c r="R77" s="73">
+        <f>R75-R73</f>
         <v>6</v>
       </c>
-      <c r="R77" s="74"/>
-      <c r="T77" s="15"/>
-    </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="S77" s="74"/>
+      <c r="U77" s="15"/>
+    </row>
+    <row r="78" spans="1:29" x14ac:dyDescent="0.3">
       <c r="C78" s="33"/>
-      <c r="T78" s="15"/>
-      <c r="Y78" s="6"/>
+      <c r="U78" s="15"/>
       <c r="Z78" s="6"/>
       <c r="AA78" s="6"/>
       <c r="AB78" s="6"/>
-    </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC78" s="6"/>
+    </row>
+    <row r="79" spans="1:29" x14ac:dyDescent="0.3">
       <c r="C79" s="33"/>
       <c r="I79" s="14"/>
       <c r="J79" s="14"/>
       <c r="K79" s="14"/>
       <c r="L79" s="14"/>
       <c r="N79" s="14"/>
-      <c r="T79" s="15"/>
-    </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U79" s="15"/>
+    </row>
+    <row r="80" spans="1:29" x14ac:dyDescent="0.3">
       <c r="C80" s="33"/>
       <c r="I80" s="14"/>
       <c r="J80" s="14"/>
       <c r="K80" s="14"/>
       <c r="L80" s="14"/>
       <c r="N80" s="14"/>
-      <c r="T80" s="15"/>
-    </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U80" s="15"/>
+    </row>
+    <row r="81" spans="1:29" x14ac:dyDescent="0.3">
       <c r="I81" s="14"/>
       <c r="J81" s="14"/>
       <c r="K81" s="14"/>
       <c r="L81" s="14"/>
       <c r="N81" s="14"/>
-      <c r="T81" s="15"/>
-    </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U81" s="15"/>
+    </row>
+    <row r="82" spans="1:29" x14ac:dyDescent="0.3">
       <c r="I82" s="14"/>
       <c r="J82" s="14"/>
       <c r="K82" s="14"/>
       <c r="L82" s="14"/>
       <c r="N82" s="14"/>
-      <c r="T82" s="15"/>
-    </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U82" s="15"/>
+    </row>
+    <row r="83" spans="1:29" x14ac:dyDescent="0.3">
       <c r="I83" s="14"/>
       <c r="J83" s="14"/>
       <c r="K83" s="14"/>
       <c r="L83" s="14"/>
       <c r="N83" s="14"/>
-      <c r="T83" s="15"/>
-      <c r="X83" s="33"/>
-    </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U83" s="15"/>
+      <c r="Y83" s="33"/>
+    </row>
+    <row r="84" spans="1:29" x14ac:dyDescent="0.3">
       <c r="I84" s="14"/>
       <c r="J84" s="14"/>
       <c r="K84" s="14"/>
       <c r="L84" s="14"/>
       <c r="N84" s="14"/>
-      <c r="T84" s="15"/>
-    </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U84" s="15"/>
+    </row>
+    <row r="85" spans="1:29" x14ac:dyDescent="0.3">
       <c r="I85" s="14"/>
       <c r="J85" s="14"/>
       <c r="K85" s="14"/>
       <c r="L85" s="14"/>
       <c r="N85" s="14"/>
     </row>
-    <row r="86" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:29" x14ac:dyDescent="0.3">
       <c r="I86" s="14"/>
       <c r="J86" s="14"/>
       <c r="K86" s="14"/>
       <c r="L86" s="14"/>
       <c r="N86" s="14"/>
     </row>
-    <row r="88" spans="1:28" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:29" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="10"/>
       <c r="B88" s="23"/>
       <c r="C88" s="14"/>
@@ -5341,74 +5450,75 @@
       <c r="O88" s="36"/>
       <c r="P88" s="36"/>
       <c r="Q88" s="36"/>
-      <c r="R88" s="2"/>
-      <c r="S88" s="3"/>
+      <c r="R88" s="36"/>
+      <c r="S88" s="2"/>
       <c r="T88" s="3"/>
       <c r="U88" s="3"/>
-      <c r="V88"/>
+      <c r="V88" s="3"/>
       <c r="W88"/>
       <c r="X88"/>
       <c r="Y88"/>
       <c r="Z88"/>
       <c r="AA88"/>
       <c r="AB88"/>
-    </row>
-    <row r="91" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="Y91" s="6"/>
+      <c r="AC88"/>
+    </row>
+    <row r="91" spans="1:29" x14ac:dyDescent="0.3">
       <c r="Z91" s="6"/>
       <c r="AA91" s="6"/>
       <c r="AB91" s="6"/>
-    </row>
-    <row r="95" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="Y95" s="6"/>
+      <c r="AC91" s="6"/>
+    </row>
+    <row r="95" spans="1:29" x14ac:dyDescent="0.3">
       <c r="Z95" s="6"/>
       <c r="AA95" s="6"/>
       <c r="AB95" s="6"/>
-    </row>
-    <row r="100" spans="25:28" x14ac:dyDescent="0.3">
-      <c r="Y100" s="6"/>
+      <c r="AC95" s="6"/>
+    </row>
+    <row r="100" spans="26:29" x14ac:dyDescent="0.3">
       <c r="Z100" s="6"/>
       <c r="AA100" s="6"/>
       <c r="AB100" s="6"/>
-    </row>
-    <row r="113" spans="25:28" x14ac:dyDescent="0.3">
-      <c r="Y113" s="33"/>
+      <c r="AC100" s="6"/>
+    </row>
+    <row r="113" spans="26:29" x14ac:dyDescent="0.3">
       <c r="Z113" s="33"/>
       <c r="AA113" s="33"/>
       <c r="AB113" s="33"/>
+      <c r="AC113" s="33"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:M70 O2:O70 Q2:S70">
+  <conditionalFormatting sqref="B2:M70 O2:O70 Q2:T70">
     <cfRule type="expression" dxfId="8" priority="37" stopIfTrue="1">
-      <formula>$S2&gt;=(0.5+$U$12)</formula>
+      <formula>$T2&gt;=(0.5+$V$12)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="7" priority="38" stopIfTrue="1">
-      <formula>$S2&gt;=$U$12</formula>
+      <formula>$T2&gt;=$V$12</formula>
     </cfRule>
     <cfRule type="expression" dxfId="6" priority="39">
-      <formula>$S2&gt;=($U$12-0.5)</formula>
+      <formula>$T2&gt;=($V$12-0.5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N70">
     <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
-      <formula>$S2&gt;=(0.5+$U$12)</formula>
+      <formula>$T2&gt;=(0.5+$V$12)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
-      <formula>$S2&gt;=$U$12</formula>
+      <formula>$T2&gt;=$V$12</formula>
     </cfRule>
     <cfRule type="expression" dxfId="3" priority="6">
-      <formula>$S2&gt;=($U$12-0.5)</formula>
+      <formula>$T2&gt;=($V$12-0.5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P70">
     <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
-      <formula>$S2&gt;=(0.5+$U$12)</formula>
+      <formula>$T2&gt;=(0.5+$V$12)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
-      <formula>$S2&gt;=$U$12</formula>
+      <formula>$T2&gt;=$V$12</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>$S2&gt;=($U$12-0.5)</formula>
+      <formula>$T2&gt;=($V$12-0.5)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>